<commit_message>
Atualizado por script em 05-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/austria_bundesliga_2023-2024.xlsx
+++ b/2023/austria_bundesliga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:V78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1401,71 +1401,71 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>A. Lustenau</t>
+          <t>BW Linz</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Austria Vienna</t>
+          <t>Hartberg</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" t="n">
-        <v>3.62</v>
+        <v>2.58</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>30/07/2023 17:12</t>
+          <t>30/07/2023 16:42</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3.93</v>
+        <v>2.31</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>06/08/2023 16:58</t>
+          <t>06/08/2023 16:59</t>
         </is>
       </c>
       <c r="N11" t="n">
-        <v>3.8</v>
+        <v>3.49</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>30/07/2023 17:12</t>
+          <t>30/07/2023 16:42</t>
         </is>
       </c>
       <c r="P11" t="n">
-        <v>3.93</v>
+        <v>3.67</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>06/08/2023 16:58</t>
+          <t>06/08/2023 16:59</t>
         </is>
       </c>
       <c r="R11" t="n">
-        <v>2.03</v>
+        <v>2.79</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>30/07/2023 17:12</t>
+          <t>30/07/2023 16:42</t>
         </is>
       </c>
       <c r="T11" t="n">
-        <v>1.93</v>
+        <v>3.09</v>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>06/08/2023 16:58</t>
+          <t>06/08/2023 16:59</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/a-lustenau-austria-vienna/0G89jgg8/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-hartberg/6FzsYpws/</t>
         </is>
       </c>
     </row>
@@ -1493,71 +1493,71 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BW Linz</t>
+          <t>A. Lustenau</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Hartberg</t>
+          <t>Austria Vienna</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" t="n">
-        <v>2.58</v>
+        <v>3.62</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>30/07/2023 16:42</t>
+          <t>30/07/2023 17:12</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>2.31</v>
+        <v>3.93</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>06/08/2023 16:59</t>
+          <t>06/08/2023 16:58</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>3.49</v>
+        <v>3.8</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>30/07/2023 16:42</t>
+          <t>30/07/2023 17:12</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>3.67</v>
+        <v>3.93</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>06/08/2023 16:59</t>
+          <t>06/08/2023 16:58</t>
         </is>
       </c>
       <c r="R12" t="n">
-        <v>2.79</v>
+        <v>2.03</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>30/07/2023 16:42</t>
+          <t>30/07/2023 17:12</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>3.09</v>
+        <v>1.93</v>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>06/08/2023 16:59</t>
+          <t>06/08/2023 16:58</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-hartberg/6FzsYpws/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/a-lustenau-austria-vienna/0G89jgg8/</t>
         </is>
       </c>
     </row>
@@ -1953,71 +1953,71 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Altach</t>
+          <t>Salzburg</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Tirol</t>
+          <t>Austria Vienna</t>
         </is>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>2.75</v>
+        <v>1.47</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>07/08/2023 07:42</t>
+          <t>06/08/2023 17:12</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2.43</v>
+        <v>1.54</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>13/08/2023 16:51</t>
+          <t>13/08/2023 16:56</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>3.52</v>
+        <v>4.94</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>07/08/2023 07:42</t>
+          <t>06/08/2023 17:12</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>3.63</v>
+        <v>4.87</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>13/08/2023 16:58</t>
+          <t>13/08/2023 16:59</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>2.56</v>
+        <v>6.21</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>07/08/2023 07:42</t>
+          <t>06/08/2023 17:12</t>
         </is>
       </c>
       <c r="T17" t="n">
-        <v>2.93</v>
+        <v>5.7</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>13/08/2023 16:51</t>
+          <t>13/08/2023 16:59</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/altach-tirol/UgL6St7I/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-austria-vienna/YRRcU2x6/</t>
         </is>
       </c>
     </row>
@@ -2045,22 +2045,22 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Salzburg</t>
+          <t>Rapid Vienna</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Austria Vienna</t>
+          <t>Hartberg</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>1.47</v>
+        <v>1.75</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -2068,15 +2068,15 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>1.54</v>
+        <v>1.93</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>13/08/2023 16:56</t>
+          <t>13/08/2023 16:57</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>4.94</v>
+        <v>4.07</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -2084,15 +2084,15 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>4.87</v>
+        <v>3.86</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>13/08/2023 16:59</t>
+          <t>13/08/2023 16:57</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>6.21</v>
+        <v>4.42</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -2100,16 +2100,16 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>5.7</v>
+        <v>3.99</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>13/08/2023 16:59</t>
+          <t>13/08/2023 16:57</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-austria-vienna/YRRcU2x6/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/rapid-vienna-hartberg/CIQ1TMiC/</t>
         </is>
       </c>
     </row>
@@ -2137,71 +2137,71 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Rapid Vienna</t>
+          <t>Altach</t>
         </is>
       </c>
       <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Tirol</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
         <v>0</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Hartberg</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>1</v>
-      </c>
       <c r="J19" t="n">
-        <v>1.75</v>
+        <v>2.75</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>06/08/2023 17:12</t>
+          <t>07/08/2023 07:42</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>1.93</v>
+        <v>2.43</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>13/08/2023 16:57</t>
+          <t>13/08/2023 16:51</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>4.07</v>
+        <v>3.52</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>06/08/2023 17:12</t>
+          <t>07/08/2023 07:42</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.86</v>
+        <v>3.63</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>13/08/2023 16:57</t>
+          <t>13/08/2023 16:58</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>4.42</v>
+        <v>2.56</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>06/08/2023 17:12</t>
+          <t>07/08/2023 07:42</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>3.99</v>
+        <v>2.93</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>13/08/2023 16:57</t>
+          <t>13/08/2023 16:51</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/rapid-vienna-hartberg/CIQ1TMiC/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/altach-tirol/UgL6St7I/</t>
         </is>
       </c>
     </row>
@@ -3057,71 +3057,71 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Hartberg</t>
+          <t>Rapid Vienna</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>A. Klagenfurt</t>
+          <t>Tirol</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J29" t="n">
-        <v>1.93</v>
+        <v>1.64</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>20/08/2023 17:12</t>
+          <t>20/08/2023 18:42</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>2.12</v>
+        <v>1.4</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>27/08/2023 16:55</t>
+          <t>27/08/2023 16:52</t>
         </is>
       </c>
       <c r="N29" t="n">
-        <v>4.13</v>
+        <v>4.37</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>20/08/2023 17:12</t>
+          <t>20/08/2023 18:42</t>
         </is>
       </c>
       <c r="P29" t="n">
-        <v>3.72</v>
+        <v>5.55</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>27/08/2023 16:55</t>
+          <t>27/08/2023 16:59</t>
         </is>
       </c>
       <c r="R29" t="n">
-        <v>3.56</v>
+        <v>5.1</v>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>20/08/2023 17:12</t>
+          <t>20/08/2023 18:42</t>
         </is>
       </c>
       <c r="T29" t="n">
-        <v>3.46</v>
+        <v>7.28</v>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>27/08/2023 16:55</t>
+          <t>27/08/2023 16:59</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/hartberg-a-klagenfurt/M5PcaNyt/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/rapid-vienna-tirol/MVhivv6U/</t>
         </is>
       </c>
     </row>
@@ -3241,71 +3241,71 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Rapid Vienna</t>
+          <t>Hartberg</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Tirol</t>
+          <t>A. Klagenfurt</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J31" t="n">
-        <v>1.64</v>
+        <v>1.93</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>20/08/2023 18:42</t>
+          <t>20/08/2023 17:12</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.4</v>
+        <v>2.12</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>27/08/2023 16:52</t>
+          <t>27/08/2023 16:55</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>4.37</v>
+        <v>4.13</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>20/08/2023 18:42</t>
+          <t>20/08/2023 17:12</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>5.55</v>
+        <v>3.72</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>27/08/2023 16:59</t>
+          <t>27/08/2023 16:55</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>5.1</v>
+        <v>3.56</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>20/08/2023 18:42</t>
+          <t>20/08/2023 17:12</t>
         </is>
       </c>
       <c r="T31" t="n">
-        <v>7.28</v>
+        <v>3.46</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>27/08/2023 16:59</t>
+          <t>27/08/2023 16:55</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/rapid-vienna-tirol/MVhivv6U/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/hartberg-a-klagenfurt/M5PcaNyt/</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Salzburg</t>
+          <t>Austria Vienna</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -3617,14 +3617,14 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Rapid Vienna</t>
+          <t>A. Klagenfurt</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J35" t="n">
-        <v>1.48</v>
+        <v>1.68</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="L35" t="n">
-        <v>1.54</v>
+        <v>1.88</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
@@ -3640,7 +3640,7 @@
         </is>
       </c>
       <c r="N35" t="n">
-        <v>4.91</v>
+        <v>4.35</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3648,7 +3648,7 @@
         </is>
       </c>
       <c r="P35" t="n">
-        <v>4.6</v>
+        <v>4.01</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
@@ -3656,7 +3656,7 @@
         </is>
       </c>
       <c r="R35" t="n">
-        <v>6.35</v>
+        <v>4.64</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
@@ -3664,7 +3664,7 @@
         </is>
       </c>
       <c r="T35" t="n">
-        <v>6.04</v>
+        <v>4</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-rapid-vienna/lIGEeuy5/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/austria-vienna-a-klagenfurt/drKMgJ5H/</t>
         </is>
       </c>
     </row>
@@ -3701,7 +3701,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>Salzburg</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -3709,14 +3709,14 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>A. Lustenau</t>
+          <t>Rapid Vienna</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1.33</v>
+        <v>1.48</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -3724,15 +3724,15 @@
         </is>
       </c>
       <c r="L36" t="n">
-        <v>1.35</v>
+        <v>1.54</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>03/09/2023 16:58</t>
+          <t>03/09/2023 16:59</t>
         </is>
       </c>
       <c r="N36" t="n">
-        <v>5.65</v>
+        <v>4.91</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3740,15 +3740,15 @@
         </is>
       </c>
       <c r="P36" t="n">
-        <v>5.73</v>
+        <v>4.6</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>03/09/2023 16:58</t>
+          <t>03/09/2023 16:59</t>
         </is>
       </c>
       <c r="R36" t="n">
-        <v>8.630000000000001</v>
+        <v>6.35</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
@@ -3756,16 +3756,16 @@
         </is>
       </c>
       <c r="T36" t="n">
-        <v>8.49</v>
+        <v>6.04</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>03/09/2023 16:58</t>
+          <t>03/09/2023 16:59</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/lask-linz-a-lustenau/S8FIfajB/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-rapid-vienna/lIGEeuy5/</t>
         </is>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Austria Vienna</t>
+          <t>LASK</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3801,14 +3801,14 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>A. Klagenfurt</t>
+          <t>A. Lustenau</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1.68</v>
+        <v>1.33</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -3816,15 +3816,15 @@
         </is>
       </c>
       <c r="L37" t="n">
-        <v>1.88</v>
+        <v>1.35</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>03/09/2023 16:59</t>
+          <t>03/09/2023 16:58</t>
         </is>
       </c>
       <c r="N37" t="n">
-        <v>4.35</v>
+        <v>5.65</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3832,15 +3832,15 @@
         </is>
       </c>
       <c r="P37" t="n">
-        <v>4.01</v>
+        <v>5.73</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>03/09/2023 16:59</t>
+          <t>03/09/2023 16:58</t>
         </is>
       </c>
       <c r="R37" t="n">
-        <v>4.64</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
@@ -3848,16 +3848,16 @@
         </is>
       </c>
       <c r="T37" t="n">
-        <v>4</v>
+        <v>8.49</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>03/09/2023 16:59</t>
+          <t>03/09/2023 16:58</t>
         </is>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/austria-vienna-a-klagenfurt/drKMgJ5H/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/lask-linz-a-lustenau/S8FIfajB/</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>BW Linz</t>
+          <t>A. Klagenfurt</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3893,14 +3893,14 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Altach</t>
+          <t>LASK</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J38" t="n">
-        <v>2.58</v>
+        <v>3.71</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -3908,15 +3908,15 @@
         </is>
       </c>
       <c r="L38" t="n">
-        <v>2.35</v>
+        <v>3.22</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>16/09/2023 16:53</t>
+          <t>16/09/2023 16:52</t>
         </is>
       </c>
       <c r="N38" t="n">
-        <v>3.62</v>
+        <v>3.88</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3924,15 +3924,15 @@
         </is>
       </c>
       <c r="P38" t="n">
-        <v>3.45</v>
+        <v>3.58</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>16/09/2023 16:53</t>
+          <t>16/09/2023 16:52</t>
         </is>
       </c>
       <c r="R38" t="n">
-        <v>2.67</v>
+        <v>1.98</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
@@ -3940,16 +3940,16 @@
         </is>
       </c>
       <c r="T38" t="n">
-        <v>3.2</v>
+        <v>2.29</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>16/09/2023 16:53</t>
+          <t>16/09/2023 16:56</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-altach/8MmuC0Lo/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/a-klagenfurt-lask-linz/Ic8ViczU/</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>A. Klagenfurt</t>
+          <t>BW Linz</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -3985,14 +3985,14 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>Altach</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J39" t="n">
-        <v>3.71</v>
+        <v>2.58</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -4000,15 +4000,15 @@
         </is>
       </c>
       <c r="L39" t="n">
-        <v>3.22</v>
+        <v>2.35</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>16/09/2023 16:52</t>
+          <t>16/09/2023 16:53</t>
         </is>
       </c>
       <c r="N39" t="n">
-        <v>3.88</v>
+        <v>3.62</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -4016,15 +4016,15 @@
         </is>
       </c>
       <c r="P39" t="n">
-        <v>3.58</v>
+        <v>3.45</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>16/09/2023 16:52</t>
+          <t>16/09/2023 16:53</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>1.98</v>
+        <v>2.67</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
@@ -4032,16 +4032,16 @@
         </is>
       </c>
       <c r="T39" t="n">
-        <v>2.29</v>
+        <v>3.2</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>16/09/2023 16:56</t>
+          <t>16/09/2023 16:53</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/a-klagenfurt-lask-linz/Ic8ViczU/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-altach/8MmuC0Lo/</t>
         </is>
       </c>
     </row>
@@ -4437,30 +4437,30 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tirol</t>
+          <t>A. Klagenfurt</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Wolfsberger AC</t>
+          <t>A. Lustenau</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>2.88</v>
+        <v>1.68</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>17/09/2023 16:13</t>
+          <t>17/09/2023 13:43</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>3.28</v>
+        <v>1.69</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
@@ -4468,15 +4468,15 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>3.62</v>
+        <v>4.12</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>17/09/2023 16:13</t>
+          <t>17/09/2023 13:43</t>
         </is>
       </c>
       <c r="P44" t="n">
-        <v>3.62</v>
+        <v>4.04</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
@@ -4484,24 +4484,24 @@
         </is>
       </c>
       <c r="R44" t="n">
-        <v>2.41</v>
+        <v>4.84</v>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>17/09/2023 16:13</t>
+          <t>17/09/2023 13:43</t>
         </is>
       </c>
       <c r="T44" t="n">
-        <v>2.24</v>
+        <v>5.17</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>23/09/2023 16:38</t>
+          <t>23/09/2023 16:50</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/tirol-wolfsberger-ac/SnnT0zDp/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/a-klagenfurt-a-lustenau/Eu6h7xzH/</t>
         </is>
       </c>
     </row>
@@ -4529,30 +4529,30 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>A. Klagenfurt</t>
+          <t>Salzburg</t>
         </is>
       </c>
       <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>BW Linz</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
         <v>1</v>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>A. Lustenau</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
-        <v>0</v>
-      </c>
       <c r="J45" t="n">
-        <v>1.68</v>
+        <v>1.16</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>17/09/2023 13:43</t>
+          <t>16/09/2023 18:42</t>
         </is>
       </c>
       <c r="L45" t="n">
-        <v>1.69</v>
+        <v>1.26</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
@@ -4560,40 +4560,40 @@
         </is>
       </c>
       <c r="N45" t="n">
-        <v>4.12</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>17/09/2023 13:43</t>
+          <t>16/09/2023 18:42</t>
         </is>
       </c>
       <c r="P45" t="n">
-        <v>4.04</v>
+        <v>6.59</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>23/09/2023 16:50</t>
+          <t>23/09/2023 16:57</t>
         </is>
       </c>
       <c r="R45" t="n">
-        <v>4.84</v>
+        <v>14.49</v>
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>17/09/2023 13:43</t>
+          <t>16/09/2023 18:42</t>
         </is>
       </c>
       <c r="T45" t="n">
-        <v>5.17</v>
+        <v>10.89</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>23/09/2023 16:50</t>
+          <t>23/09/2023 16:57</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/a-klagenfurt-a-lustenau/Eu6h7xzH/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-bw-linz/6F2p9b54/</t>
         </is>
       </c>
     </row>
@@ -4621,30 +4621,30 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Salzburg</t>
+          <t>Tirol</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>BW Linz</t>
+          <t>Wolfsberger AC</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J46" t="n">
-        <v>1.16</v>
+        <v>2.88</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>16/09/2023 18:42</t>
+          <t>17/09/2023 16:13</t>
         </is>
       </c>
       <c r="L46" t="n">
-        <v>1.26</v>
+        <v>3.28</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
@@ -4652,40 +4652,40 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>8.359999999999999</v>
+        <v>3.62</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>16/09/2023 18:42</t>
+          <t>17/09/2023 16:13</t>
         </is>
       </c>
       <c r="P46" t="n">
-        <v>6.59</v>
+        <v>3.62</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>23/09/2023 16:57</t>
+          <t>23/09/2023 16:50</t>
         </is>
       </c>
       <c r="R46" t="n">
-        <v>14.49</v>
+        <v>2.41</v>
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>16/09/2023 18:42</t>
+          <t>17/09/2023 16:13</t>
         </is>
       </c>
       <c r="T46" t="n">
-        <v>10.89</v>
+        <v>2.24</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>23/09/2023 16:57</t>
+          <t>23/09/2023 16:38</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-bw-linz/6F2p9b54/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/tirol-wolfsberger-ac/SnnT0zDp/</t>
         </is>
       </c>
     </row>
@@ -4713,22 +4713,22 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>Altach</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Hartberg</t>
+          <t>Austria Vienna</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>1.59</v>
+        <v>3.58</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -4736,7 +4736,7 @@
         </is>
       </c>
       <c r="L47" t="n">
-        <v>1.74</v>
+        <v>2.95</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
@@ -4744,7 +4744,7 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>4.48</v>
+        <v>3.87</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4752,7 +4752,7 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>4.17</v>
+        <v>3.53</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
@@ -4760,7 +4760,7 @@
         </is>
       </c>
       <c r="R47" t="n">
-        <v>5.48</v>
+        <v>1.99</v>
       </c>
       <c r="S47" t="inlineStr">
         <is>
@@ -4768,16 +4768,16 @@
         </is>
       </c>
       <c r="T47" t="n">
-        <v>4.62</v>
+        <v>2.47</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>24/09/2023 14:14</t>
+          <t>24/09/2023 14:29</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/lask-linz-hartberg/0x2l8IKA/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/altach-austria-vienna/zef15G4T/</t>
         </is>
       </c>
     </row>
@@ -4805,22 +4805,22 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Altach</t>
+          <t>LASK</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Austria Vienna</t>
+          <t>Hartberg</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>3.58</v>
+        <v>1.59</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -4828,7 +4828,7 @@
         </is>
       </c>
       <c r="L48" t="n">
-        <v>2.95</v>
+        <v>1.74</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
@@ -4836,7 +4836,7 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>3.87</v>
+        <v>4.48</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4844,7 +4844,7 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>3.53</v>
+        <v>4.17</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
@@ -4852,7 +4852,7 @@
         </is>
       </c>
       <c r="R48" t="n">
-        <v>1.99</v>
+        <v>5.48</v>
       </c>
       <c r="S48" t="inlineStr">
         <is>
@@ -4860,16 +4860,16 @@
         </is>
       </c>
       <c r="T48" t="n">
-        <v>2.47</v>
+        <v>4.62</v>
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>24/09/2023 14:29</t>
+          <t>24/09/2023 14:14</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/altach-austria-vienna/zef15G4T/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/lask-linz-hartberg/0x2l8IKA/</t>
         </is>
       </c>
     </row>
@@ -4989,71 +4989,71 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>A. Lustenau</t>
+          <t>Wolfsberger AC</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Salzburg</t>
+          <t>LASK</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>9.880000000000001</v>
+        <v>3.3</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 13:42</t>
         </is>
       </c>
       <c r="L50" t="n">
-        <v>13.38</v>
+        <v>3.19</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>30/09/2023 16:48</t>
+          <t>30/09/2023 16:43</t>
         </is>
       </c>
       <c r="N50" t="n">
-        <v>6.64</v>
+        <v>3.73</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 13:42</t>
         </is>
       </c>
       <c r="P50" t="n">
-        <v>7.85</v>
+        <v>3.44</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>30/09/2023 16:48</t>
+          <t>30/09/2023 16:59</t>
         </is>
       </c>
       <c r="R50" t="n">
-        <v>1.25</v>
+        <v>2.13</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>23/09/2023 17:13</t>
+          <t>24/09/2023 13:42</t>
         </is>
       </c>
       <c r="T50" t="n">
-        <v>1.2</v>
+        <v>2.35</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>30/09/2023 16:34</t>
+          <t>30/09/2023 16:43</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/a-lustenau-salzburg/vstRLykA/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/wolfsberger-ac-lask-linz/6woXafSj/</t>
         </is>
       </c>
     </row>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>BW Linz</t>
+          <t>A. Lustenau</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -5089,14 +5089,14 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>A. Klagenfurt</t>
+          <t>Salzburg</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J51" t="n">
-        <v>2.81</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,15 +5104,15 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>2.7</v>
+        <v>13.38</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>30/09/2023 16:50</t>
+          <t>30/09/2023 16:48</t>
         </is>
       </c>
       <c r="N51" t="n">
-        <v>3.54</v>
+        <v>6.64</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,15 +5120,15 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>3.38</v>
+        <v>7.85</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>30/09/2023 16:38</t>
+          <t>30/09/2023 16:48</t>
         </is>
       </c>
       <c r="R51" t="n">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,16 +5136,16 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>2.77</v>
+        <v>1.2</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>30/09/2023 16:50</t>
+          <t>30/09/2023 16:34</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-a-klagenfurt/0jsNMHZ3/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/a-lustenau-salzburg/vstRLykA/</t>
         </is>
       </c>
     </row>
@@ -5173,71 +5173,71 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Wolfsberger AC</t>
+          <t>BW Linz</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>A. Klagenfurt</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>3.3</v>
+        <v>2.81</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>24/09/2023 13:42</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="L52" t="n">
-        <v>3.19</v>
+        <v>2.7</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>30/09/2023 16:43</t>
+          <t>30/09/2023 16:50</t>
         </is>
       </c>
       <c r="N52" t="n">
-        <v>3.73</v>
+        <v>3.54</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>24/09/2023 13:42</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="P52" t="n">
-        <v>3.44</v>
+        <v>3.38</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>30/09/2023 16:59</t>
+          <t>30/09/2023 16:38</t>
         </is>
       </c>
       <c r="R52" t="n">
-        <v>2.13</v>
+        <v>2.5</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>24/09/2023 13:42</t>
+          <t>23/09/2023 17:13</t>
         </is>
       </c>
       <c r="T52" t="n">
-        <v>2.35</v>
+        <v>2.77</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>30/09/2023 16:43</t>
+          <t>30/09/2023 16:50</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/wolfsberger-ac-lask-linz/6woXafSj/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-a-klagenfurt/0jsNMHZ3/</t>
         </is>
       </c>
     </row>
@@ -5541,71 +5541,71 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Hartberg</t>
+          <t>A. Lustenau</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Tirol</t>
+          <t>Rapid Vienna</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J56" t="n">
-        <v>1.61</v>
+        <v>5.42</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>01/10/2023 13:42</t>
+          <t>01/10/2023 16:12</t>
         </is>
       </c>
       <c r="L56" t="n">
-        <v>1.6</v>
+        <v>7.27</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>07/10/2023 16:55</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="N56" t="n">
-        <v>4.4</v>
+        <v>4.45</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>01/10/2023 13:42</t>
+          <t>01/10/2023 16:12</t>
         </is>
       </c>
       <c r="P56" t="n">
-        <v>4.43</v>
+        <v>5.21</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>07/10/2023 16:46</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="R56" t="n">
-        <v>5.12</v>
+        <v>1.57</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
-          <t>01/10/2023 13:42</t>
+          <t>01/10/2023 16:12</t>
         </is>
       </c>
       <c r="T56" t="n">
-        <v>5.5</v>
+        <v>1.42</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>07/10/2023 16:55</t>
+          <t>07/10/2023 16:42</t>
         </is>
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/hartberg-tirol/UTwbOUA8/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/a-lustenau-rapid-vienna/2NkGaoY7/</t>
         </is>
       </c>
     </row>
@@ -5725,71 +5725,71 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>A. Lustenau</t>
+          <t>Hartberg</t>
         </is>
       </c>
       <c r="G58" t="n">
+        <v>3</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Tirol</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
         <v>0</v>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Rapid Vienna</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>5</v>
-      </c>
       <c r="J58" t="n">
-        <v>5.42</v>
+        <v>1.61</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>01/10/2023 16:12</t>
+          <t>01/10/2023 13:42</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>7.27</v>
+        <v>1.6</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 16:55</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>4.45</v>
+        <v>4.4</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>01/10/2023 16:12</t>
+          <t>01/10/2023 13:42</t>
         </is>
       </c>
       <c r="P58" t="n">
-        <v>5.21</v>
+        <v>4.43</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 16:46</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>1.57</v>
+        <v>5.12</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>01/10/2023 16:12</t>
+          <t>01/10/2023 13:42</t>
         </is>
       </c>
       <c r="T58" t="n">
-        <v>1.42</v>
+        <v>5.5</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>07/10/2023 16:42</t>
+          <t>07/10/2023 16:55</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/a-lustenau-rapid-vienna/2NkGaoY7/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/hartberg-tirol/UTwbOUA8/</t>
         </is>
       </c>
     </row>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>Wolfsberger AC</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -5825,14 +5825,14 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Altach</t>
+          <t>Sturm Graz</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J59" t="n">
-        <v>1.46</v>
+        <v>4.32</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
@@ -5840,15 +5840,15 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>1.84</v>
+        <v>4.28</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>08/10/2023 14:10</t>
+          <t>08/10/2023 14:21</t>
         </is>
       </c>
       <c r="N59" t="n">
-        <v>4.72</v>
+        <v>4.03</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5856,15 +5856,15 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>3.69</v>
+        <v>3.83</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>08/10/2023 14:27</t>
+          <t>08/10/2023 14:21</t>
         </is>
       </c>
       <c r="R59" t="n">
-        <v>6.77</v>
+        <v>1.78</v>
       </c>
       <c r="S59" t="inlineStr">
         <is>
@@ -5872,16 +5872,16 @@
         </is>
       </c>
       <c r="T59" t="n">
-        <v>4.63</v>
+        <v>1.87</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>08/10/2023 14:27</t>
+          <t>08/10/2023 14:21</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/lask-linz-altach/Ysba3TYr/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/wolfsberger-ac-sturm-graz/S4c32mlk/</t>
         </is>
       </c>
     </row>
@@ -5909,7 +5909,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Wolfsberger AC</t>
+          <t>LASK</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -5917,14 +5917,14 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Sturm Graz</t>
+          <t>Altach</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>4.32</v>
+        <v>1.46</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -5932,15 +5932,15 @@
         </is>
       </c>
       <c r="L60" t="n">
-        <v>4.28</v>
+        <v>1.84</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>08/10/2023 14:21</t>
+          <t>08/10/2023 14:10</t>
         </is>
       </c>
       <c r="N60" t="n">
-        <v>4.03</v>
+        <v>4.72</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -5948,15 +5948,15 @@
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.83</v>
+        <v>3.69</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>08/10/2023 14:21</t>
+          <t>08/10/2023 14:27</t>
         </is>
       </c>
       <c r="R60" t="n">
-        <v>1.78</v>
+        <v>6.77</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
@@ -5964,16 +5964,16 @@
         </is>
       </c>
       <c r="T60" t="n">
-        <v>1.87</v>
+        <v>4.63</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>08/10/2023 14:21</t>
+          <t>08/10/2023 14:27</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/wolfsberger-ac-sturm-graz/S4c32mlk/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/lask-linz-altach/Ysba3TYr/</t>
         </is>
       </c>
     </row>
@@ -6645,71 +6645,71 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>A. Klagenfurt</t>
+          <t>Salzburg</t>
         </is>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Tirol</t>
+          <t>Altach</t>
         </is>
       </c>
       <c r="I68" t="n">
         <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>1.62</v>
+        <v>1.17</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>22/10/2023 17:12</t>
+          <t>22/10/2023 14:42</t>
         </is>
       </c>
       <c r="L68" t="n">
-        <v>1.79</v>
+        <v>1.27</v>
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>28/10/2023 16:59</t>
+          <t>28/10/2023 16:38</t>
         </is>
       </c>
       <c r="N68" t="n">
-        <v>4.26</v>
+        <v>7.81</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>22/10/2023 17:12</t>
+          <t>22/10/2023 14:42</t>
         </is>
       </c>
       <c r="P68" t="n">
-        <v>3.89</v>
+        <v>6.39</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>28/10/2023 16:59</t>
+          <t>28/10/2023 16:52</t>
         </is>
       </c>
       <c r="R68" t="n">
-        <v>5.25</v>
+        <v>16.28</v>
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>22/10/2023 17:12</t>
+          <t>22/10/2023 14:42</t>
         </is>
       </c>
       <c r="T68" t="n">
-        <v>4.65</v>
+        <v>11.39</v>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>28/10/2023 16:59</t>
+          <t>28/10/2023 16:52</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/a-klagenfurt-tirol/2sEcCOHD/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-altach/dpBkEpm1/</t>
         </is>
       </c>
     </row>
@@ -6737,71 +6737,71 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>BW Linz</t>
+          <t>A. Klagenfurt</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Wolfsberger AC</t>
+          <t>Tirol</t>
         </is>
       </c>
       <c r="I69" t="n">
         <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>2.63</v>
+        <v>1.62</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>22/10/2023 14:42</t>
+          <t>22/10/2023 17:12</t>
         </is>
       </c>
       <c r="L69" t="n">
-        <v>2.76</v>
+        <v>1.79</v>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>28/10/2023 16:56</t>
+          <t>28/10/2023 16:59</t>
         </is>
       </c>
       <c r="N69" t="n">
-        <v>3.55</v>
+        <v>4.26</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>22/10/2023 14:42</t>
+          <t>22/10/2023 17:12</t>
         </is>
       </c>
       <c r="P69" t="n">
-        <v>3.43</v>
+        <v>3.89</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>28/10/2023 16:52</t>
+          <t>28/10/2023 16:59</t>
         </is>
       </c>
       <c r="R69" t="n">
-        <v>2.71</v>
+        <v>5.25</v>
       </c>
       <c r="S69" t="inlineStr">
         <is>
-          <t>22/10/2023 14:42</t>
+          <t>22/10/2023 17:12</t>
         </is>
       </c>
       <c r="T69" t="n">
-        <v>2.68</v>
+        <v>4.65</v>
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>28/10/2023 16:53</t>
+          <t>28/10/2023 16:59</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-wolfsberger-ac/p6wrKzyK/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/a-klagenfurt-tirol/2sEcCOHD/</t>
         </is>
       </c>
     </row>
@@ -6829,22 +6829,22 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Salzburg</t>
+          <t>BW Linz</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Altach</t>
+          <t>Wolfsberger AC</t>
         </is>
       </c>
       <c r="I70" t="n">
         <v>0</v>
       </c>
       <c r="J70" t="n">
-        <v>1.17</v>
+        <v>2.63</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
@@ -6852,15 +6852,15 @@
         </is>
       </c>
       <c r="L70" t="n">
-        <v>1.27</v>
+        <v>2.76</v>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>28/10/2023 16:38</t>
+          <t>28/10/2023 16:56</t>
         </is>
       </c>
       <c r="N70" t="n">
-        <v>7.81</v>
+        <v>3.55</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -6868,7 +6868,7 @@
         </is>
       </c>
       <c r="P70" t="n">
-        <v>6.39</v>
+        <v>3.43</v>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
@@ -6876,7 +6876,7 @@
         </is>
       </c>
       <c r="R70" t="n">
-        <v>16.28</v>
+        <v>2.71</v>
       </c>
       <c r="S70" t="inlineStr">
         <is>
@@ -6884,16 +6884,16 @@
         </is>
       </c>
       <c r="T70" t="n">
-        <v>11.39</v>
+        <v>2.68</v>
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>28/10/2023 16:52</t>
+          <t>28/10/2023 16:53</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/salzburg-altach/dpBkEpm1/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/bw-linz-wolfsberger-ac/p6wrKzyK/</t>
         </is>
       </c>
     </row>
@@ -7197,71 +7197,71 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Tirol</t>
+          <t>Austria Vienna</t>
         </is>
       </c>
       <c r="G74" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>A. Lustenau</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
         <v>0</v>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Salzburg</t>
-        </is>
-      </c>
-      <c r="I74" t="n">
-        <v>2</v>
-      </c>
       <c r="J74" t="n">
-        <v>8.32</v>
+        <v>1.37</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>28/10/2023 18:12</t>
+          <t>29/10/2023 14:42</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>11.61</v>
+        <v>1.28</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>04/11/2023 16:44</t>
+          <t>04/11/2023 16:54</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>5.55</v>
+        <v>5.29</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>28/10/2023 18:12</t>
+          <t>29/10/2023 14:42</t>
         </is>
       </c>
       <c r="P74" t="n">
-        <v>6.58</v>
+        <v>6.23</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>04/11/2023 16:48</t>
+          <t>04/11/2023 16:56</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>1.36</v>
+        <v>7.99</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>28/10/2023 18:12</t>
+          <t>29/10/2023 14:42</t>
         </is>
       </c>
       <c r="T74" t="n">
-        <v>1.25</v>
+        <v>10.31</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>04/11/2023 14:52</t>
+          <t>04/11/2023 16:56</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/tirol-salzburg/CjhR9jDC/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/austria-vienna-a-lustenau/CGNMChTg/</t>
         </is>
       </c>
     </row>
@@ -7289,71 +7289,71 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Austria Vienna</t>
+          <t>Tirol</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>A. Lustenau</t>
+          <t>Salzburg</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J75" t="n">
-        <v>1.37</v>
+        <v>8.32</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>29/10/2023 14:42</t>
+          <t>28/10/2023 18:12</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>1.28</v>
+        <v>11.61</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>04/11/2023 16:54</t>
+          <t>04/11/2023 16:44</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>5.29</v>
+        <v>5.55</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>29/10/2023 14:42</t>
+          <t>28/10/2023 18:12</t>
         </is>
       </c>
       <c r="P75" t="n">
-        <v>6.23</v>
+        <v>6.58</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>04/11/2023 16:56</t>
+          <t>04/11/2023 16:48</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>7.99</v>
+        <v>1.36</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
-          <t>29/10/2023 14:42</t>
+          <t>28/10/2023 18:12</t>
         </is>
       </c>
       <c r="T75" t="n">
-        <v>10.31</v>
+        <v>1.25</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>04/11/2023 16:56</t>
+          <t>04/11/2023 14:52</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/austria/bundesliga/austria-vienna-a-lustenau/CGNMChTg/</t>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/tirol-salzburg/CjhR9jDC/</t>
         </is>
       </c>
     </row>
@@ -7446,6 +7446,190 @@
       <c r="V76" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/austria/bundesliga/wolfsberger-ac-a-klagenfurt/bDJIDYDm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>austria</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>bundesliga</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>45235.60416666666</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Altach</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Rapid Vienna</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>2</v>
+      </c>
+      <c r="J77" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>29/10/2023 17:12</t>
+        </is>
+      </c>
+      <c r="L77" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>05/11/2023 14:27</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>29/10/2023 17:12</t>
+        </is>
+      </c>
+      <c r="P77" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>05/11/2023 14:27</t>
+        </is>
+      </c>
+      <c r="R77" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>29/10/2023 17:12</t>
+        </is>
+      </c>
+      <c r="T77" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>05/11/2023 14:27</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/altach-rapid-vienna/6wNQBCr0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>austria</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>bundesliga</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>45235.60416666666</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Hartberg</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>3</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>BW Linz</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>2</v>
+      </c>
+      <c r="J78" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>29/10/2023 14:42</t>
+        </is>
+      </c>
+      <c r="L78" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>05/11/2023 14:29</t>
+        </is>
+      </c>
+      <c r="N78" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>29/10/2023 14:42</t>
+        </is>
+      </c>
+      <c r="P78" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>05/11/2023 14:29</t>
+        </is>
+      </c>
+      <c r="R78" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>29/10/2023 14:42</t>
+        </is>
+      </c>
+      <c r="T78" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>05/11/2023 14:29</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/austria/bundesliga/hartberg-bw-linz/pULUAWc6/</t>
         </is>
       </c>
     </row>

</xml_diff>